<commit_message>
Added open dialogue query and popup
</commit_message>
<xml_diff>
--- a/misc/database/mainDB.xlsx
+++ b/misc/database/mainDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sibusiso\source\repos\QuantIO\misc\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B41C13-2A49-4689-BEA9-AE7343E00A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E19DECC-2F82-490E-978B-C74A1E2C83AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1540,7 +1540,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added currency popup details
</commit_message>
<xml_diff>
--- a/misc/database/mainDB.xlsx
+++ b/misc/database/mainDB.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sibusiso\source\repos\QuantIO\misc\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E19DECC-2F82-490E-978B-C74A1E2C83AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8DCD1F-1F09-4D9D-A03E-DBECA68D07CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1536,11 +1536,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3742,10 +3743,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2432AD31-1E99-410E-89F7-182EE6D23D28}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3881,13 +3883,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92EB9BD-10F7-4BB8-8965-84B9D99E1299}">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4077,6 +4079,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EE4064-89D3-48CC-B9FA-4C8139C423E6}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Currency edit and read only mode
</commit_message>
<xml_diff>
--- a/misc/database/mainDB.xlsx
+++ b/misc/database/mainDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sibusiso\source\repos\QuantIO\misc\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8DCD1F-1F09-4D9D-A03E-DBECA68D07CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460781AE-FB59-440A-B32F-23750EC37427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CURRENCIES" sheetId="1" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
@@ -3888,8 +3888,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>